<commit_message>
Fixed bug in POWER data processing
</commit_message>
<xml_diff>
--- a/Code/Inputs/Power_curve.xlsx
+++ b/Code/Inputs/Power_curve.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivans\Desktop\TESI\MicroGridsPy-SESAM-MYCE\Code\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivans\Desktop\TESI\On-grid\MicroGridsPy-OnGrid\One building - National Grid\MicroGridsPy-SESAM-MYCE _to be used\MicroGridsPy-SESAM-MYCE\Code\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491FBEAA-C514-48E3-A1A3-6709811C4637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFB78A5-6E03-41FE-AF1B-3C0B63B106D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{583D8F24-B3C1-4AD9-AD31-0D39345084B6}"/>
   </bookViews>
@@ -75,7 +75,7 @@
     <t>&lt;-- Fill in with turbine data according to the example in col. B</t>
   </si>
   <si>
-    <t>Bonus.B23.150</t>
+    <t>NPS100c-21</t>
   </si>
 </sst>
 </file>
@@ -184,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -193,29 +193,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -310,15 +328,15 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$B$1</c:f>
+              <c:f>Foglio1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Alstom.Eco.80 (example)</c:v>
+                  <c:v>NPS100c-21</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -326,7 +344,7 @@
           <c:spPr>
             <a:ln w="22225" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -436,237 +454,6 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$B$6:$B$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.5049999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>39.244999999999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>107.715</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>211.255</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>354.03999999999996</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>543.58500000000004</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>787.40499999999997</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1063.79</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1342.68</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1558.1100000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1652.4650000000001</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1670</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1670</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1670</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1670</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1648.29</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1596.52</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1547.2549999999999</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1498.825</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1449.56</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1400.2950000000001</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1351.865</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1302.6000000000001</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7B7F-4D64-A6DD-77956168C675}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Foglio1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Bonus.B23.150</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Foglio1!$A$6:$A$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
               <c:f>Foglio1!$C$6:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -681,73 +468,73 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.851851851851855</c:v>
+                  <c:v>4.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.623781676413261</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.929824561403549</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34.795321637426852</c:v>
+                  <c:v>29.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>57.017543859649052</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>81.481481481481495</c:v>
+                  <c:v>54.3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>106.53021442495125</c:v>
+                  <c:v>66.8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>127.68031189083825</c:v>
+                  <c:v>77.7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>142.30019493177392</c:v>
+                  <c:v>86.4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>149.90253411306045</c:v>
+                  <c:v>92.8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>150</c:v>
+                  <c:v>97.8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>144.83430799220267</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>136.1598440545809</c:v>
+                  <c:v>99.9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>127.58284600389871</c:v>
+                  <c:v>99.2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>121.24756335282646</c:v>
+                  <c:v>98.4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>117.44639376218325</c:v>
+                  <c:v>97.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>115.6920077972709</c:v>
+                  <c:v>96.8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>115.20467836257315</c:v>
+                  <c:v>96.4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>114.71734892787525</c:v>
+                  <c:v>96.3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>114.52241715399616</c:v>
+                  <c:v>96.8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>114.42495126705646</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>114.52241715399616</c:v>
+                  <c:v>99.2</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0</c:v>
@@ -3007,15 +2794,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3378,456 +3165,454 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BD5D45-96B0-4B86-9518-8D7C56B645E0}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" customWidth="1"/>
-    <col min="4" max="4" width="56.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="56" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="18">
         <v>1670</v>
       </c>
-      <c r="C2" s="17">
-        <v>150</v>
-      </c>
-      <c r="D2" s="19"/>
+      <c r="C2" s="19">
+        <v>100</v>
+      </c>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="18">
         <v>80</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="19">
+        <v>20.7</v>
+      </c>
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18">
+        <v>80</v>
+      </c>
+      <c r="C4" s="19">
+        <v>37</v>
+      </c>
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="23">
+        <v>0</v>
+      </c>
+      <c r="B6" s="22">
+        <v>0</v>
+      </c>
+      <c r="C6" s="22">
+        <v>0</v>
+      </c>
+      <c r="D6" s="13"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="23">
+        <v>1</v>
+      </c>
+      <c r="B7" s="22">
+        <v>0</v>
+      </c>
+      <c r="C7" s="22">
+        <v>0</v>
+      </c>
+      <c r="D7" s="13"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="23">
+        <v>2</v>
+      </c>
+      <c r="B8" s="22">
+        <v>0</v>
+      </c>
+      <c r="C8" s="22">
+        <v>0</v>
+      </c>
+      <c r="D8" s="13"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="23">
+        <v>3</v>
+      </c>
+      <c r="B9" s="22">
+        <v>2.5049999999999999</v>
+      </c>
+      <c r="C9" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="13"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="23">
+        <v>4</v>
+      </c>
+      <c r="B10" s="22">
+        <v>39.244999999999997</v>
+      </c>
+      <c r="C10" s="22">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D10" s="13"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="23">
+        <v>5</v>
+      </c>
+      <c r="B11" s="22">
+        <v>107.715</v>
+      </c>
+      <c r="C11" s="22">
+        <v>10.5</v>
+      </c>
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="23">
+        <v>6</v>
+      </c>
+      <c r="B12" s="22">
+        <v>211.255</v>
+      </c>
+      <c r="C12" s="22">
+        <v>19</v>
+      </c>
+      <c r="D12" s="13"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="23">
+        <v>7</v>
+      </c>
+      <c r="B13" s="22">
+        <v>354.03999999999996</v>
+      </c>
+      <c r="C13" s="22">
+        <v>29.4</v>
+      </c>
+      <c r="D13" s="13"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="23">
+        <v>8</v>
+      </c>
+      <c r="B14" s="22">
+        <v>543.58500000000004</v>
+      </c>
+      <c r="C14" s="22">
+        <v>41</v>
+      </c>
+      <c r="D14" s="13"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="23">
+        <v>9</v>
+      </c>
+      <c r="B15" s="22">
+        <v>787.40499999999997</v>
+      </c>
+      <c r="C15" s="22">
+        <v>54.3</v>
+      </c>
+      <c r="D15" s="13"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="23">
+        <v>10</v>
+      </c>
+      <c r="B16" s="22">
+        <v>1063.79</v>
+      </c>
+      <c r="C16" s="22">
+        <v>66.8</v>
+      </c>
+      <c r="D16" s="13"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="23">
+        <v>11</v>
+      </c>
+      <c r="B17" s="22">
+        <v>1342.68</v>
+      </c>
+      <c r="C17" s="22">
+        <v>77.7</v>
+      </c>
+      <c r="D17" s="13"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="23">
+        <v>12</v>
+      </c>
+      <c r="B18" s="22">
+        <v>1558.1100000000001</v>
+      </c>
+      <c r="C18" s="22">
+        <v>86.4</v>
+      </c>
+      <c r="D18" s="13"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="23">
+        <v>13</v>
+      </c>
+      <c r="B19" s="22">
+        <v>1652.4650000000001</v>
+      </c>
+      <c r="C19" s="22">
+        <v>92.8</v>
+      </c>
+      <c r="D19" s="13"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="23">
+        <v>14</v>
+      </c>
+      <c r="B20" s="22">
+        <v>1670</v>
+      </c>
+      <c r="C20" s="22">
+        <v>97.8</v>
+      </c>
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="23">
+        <v>15</v>
+      </c>
+      <c r="B21" s="22">
+        <v>1670</v>
+      </c>
+      <c r="C21" s="22">
+        <v>100</v>
+      </c>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="23">
+        <v>16</v>
+      </c>
+      <c r="B22" s="22">
+        <v>1670</v>
+      </c>
+      <c r="C22" s="22">
+        <v>99.9</v>
+      </c>
+      <c r="D22" s="13"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="23">
+        <v>17</v>
+      </c>
+      <c r="B23" s="22">
+        <v>1670</v>
+      </c>
+      <c r="C23" s="22">
+        <v>99.2</v>
+      </c>
+      <c r="D23" s="13"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="23">
+        <v>18</v>
+      </c>
+      <c r="B24" s="22">
+        <v>1648.29</v>
+      </c>
+      <c r="C24" s="22">
+        <v>98.4</v>
+      </c>
+      <c r="D24" s="13"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="23">
+        <v>19</v>
+      </c>
+      <c r="B25" s="22">
+        <v>1596.52</v>
+      </c>
+      <c r="C25" s="22">
+        <v>97.5</v>
+      </c>
+      <c r="D25" s="13"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="23">
+        <v>20</v>
+      </c>
+      <c r="B26" s="22">
+        <v>1547.2549999999999</v>
+      </c>
+      <c r="C26" s="22">
+        <v>96.8</v>
+      </c>
+      <c r="D26" s="13"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="23">
+        <v>21</v>
+      </c>
+      <c r="B27" s="22">
+        <v>1498.825</v>
+      </c>
+      <c r="C27" s="22">
+        <v>96.4</v>
+      </c>
+      <c r="D27" s="13"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="23">
+        <v>22</v>
+      </c>
+      <c r="B28" s="22">
+        <v>1449.56</v>
+      </c>
+      <c r="C28" s="22">
+        <v>96.3</v>
+      </c>
+      <c r="D28" s="13"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="23">
         <v>23</v>
       </c>
-      <c r="D3" s="19"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="16">
-        <v>80</v>
-      </c>
-      <c r="C4" s="17">
-        <v>40</v>
-      </c>
-      <c r="D4" s="19"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="19"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="19"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" s="19"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8" s="19"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>3</v>
-      </c>
-      <c r="B9">
-        <v>2.5049999999999999</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9" s="19"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>4</v>
-      </c>
-      <c r="B10">
-        <v>39.244999999999997</v>
-      </c>
-      <c r="C10">
-        <v>1.851851851851855</v>
-      </c>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="B29" s="22">
+        <v>1400.2950000000001</v>
+      </c>
+      <c r="C29" s="22">
+        <v>96.8</v>
+      </c>
+      <c r="D29" s="13"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="23">
+        <v>24</v>
+      </c>
+      <c r="B30" s="22">
+        <v>1351.865</v>
+      </c>
+      <c r="C30" s="22">
+        <v>98</v>
+      </c>
+      <c r="D30" s="13"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="23">
+        <v>25</v>
+      </c>
+      <c r="B31" s="22">
+        <v>1302.6000000000001</v>
+      </c>
+      <c r="C31" s="22">
+        <v>99.2</v>
+      </c>
+      <c r="D31" s="13"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="23">
+        <v>26</v>
+      </c>
+      <c r="B32" s="22">
+        <v>0</v>
+      </c>
+      <c r="C32" s="22">
+        <v>0</v>
+      </c>
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="23">
+        <v>27</v>
+      </c>
+      <c r="B33" s="22">
+        <v>0</v>
+      </c>
+      <c r="C33" s="22">
+        <v>0</v>
+      </c>
+      <c r="D33" s="13"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="23">
+        <v>28</v>
+      </c>
+      <c r="B34" s="22">
+        <v>0</v>
+      </c>
+      <c r="C34" s="22">
+        <v>0</v>
+      </c>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="23">
+        <v>29</v>
+      </c>
+      <c r="B35" s="22">
+        <v>0</v>
+      </c>
+      <c r="C35" s="22">
+        <v>0</v>
+      </c>
+      <c r="D35" s="13"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="D36" s="9"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B11">
-        <v>107.715</v>
-      </c>
-      <c r="C11">
-        <v>10.623781676413261</v>
-      </c>
-      <c r="D11" s="19"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>211.255</v>
-      </c>
-      <c r="C12">
-        <v>21.929824561403549</v>
-      </c>
-      <c r="D12" s="19"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>354.03999999999996</v>
-      </c>
-      <c r="C13">
-        <v>34.795321637426852</v>
-      </c>
-      <c r="D13" s="19"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>8</v>
-      </c>
-      <c r="B14">
-        <v>543.58500000000004</v>
-      </c>
-      <c r="C14">
-        <v>57.017543859649052</v>
-      </c>
-      <c r="D14" s="19"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>9</v>
-      </c>
-      <c r="B15">
-        <v>787.40499999999997</v>
-      </c>
-      <c r="C15">
-        <v>81.481481481481495</v>
-      </c>
-      <c r="D15" s="19"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="B37" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B16">
-        <v>1063.79</v>
-      </c>
-      <c r="C16">
-        <v>106.53021442495125</v>
-      </c>
-      <c r="D16" s="19"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>11</v>
-      </c>
-      <c r="B17">
-        <v>1342.68</v>
-      </c>
-      <c r="C17">
-        <v>127.68031189083825</v>
-      </c>
-      <c r="D17" s="19"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>12</v>
-      </c>
-      <c r="B18">
-        <v>1558.1100000000001</v>
-      </c>
-      <c r="C18">
-        <v>142.30019493177392</v>
-      </c>
-      <c r="D18" s="19"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>13</v>
-      </c>
-      <c r="B19">
-        <v>1652.4650000000001</v>
-      </c>
-      <c r="C19">
-        <v>149.90253411306045</v>
-      </c>
-      <c r="D19" s="19"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>14</v>
-      </c>
-      <c r="B20">
-        <v>1670</v>
-      </c>
-      <c r="C20">
-        <v>150</v>
-      </c>
-      <c r="D20" s="19"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>15</v>
-      </c>
-      <c r="B21">
-        <v>1670</v>
-      </c>
-      <c r="C21">
-        <v>144.83430799220267</v>
-      </c>
-      <c r="D21" s="19"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>16</v>
-      </c>
-      <c r="B22">
-        <v>1670</v>
-      </c>
-      <c r="C22">
-        <v>136.1598440545809</v>
-      </c>
-      <c r="D22" s="19"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>17</v>
-      </c>
-      <c r="B23">
-        <v>1670</v>
-      </c>
-      <c r="C23">
-        <v>127.58284600389871</v>
-      </c>
-      <c r="D23" s="19"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>18</v>
-      </c>
-      <c r="B24">
-        <v>1648.29</v>
-      </c>
-      <c r="C24">
-        <v>121.24756335282646</v>
-      </c>
-      <c r="D24" s="19"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>19</v>
-      </c>
-      <c r="B25">
-        <v>1596.52</v>
-      </c>
-      <c r="C25">
-        <v>117.44639376218325</v>
-      </c>
-      <c r="D25" s="19"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>20</v>
-      </c>
-      <c r="B26">
-        <v>1547.2549999999999</v>
-      </c>
-      <c r="C26">
-        <v>115.6920077972709</v>
-      </c>
-      <c r="D26" s="19"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>21</v>
-      </c>
-      <c r="B27">
-        <v>1498.825</v>
-      </c>
-      <c r="C27">
-        <v>115.20467836257315</v>
-      </c>
-      <c r="D27" s="19"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>22</v>
-      </c>
-      <c r="B28">
-        <v>1449.56</v>
-      </c>
-      <c r="C28">
-        <v>114.71734892787525</v>
-      </c>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>23</v>
-      </c>
-      <c r="B29">
-        <v>1400.2950000000001</v>
-      </c>
-      <c r="C29">
-        <v>114.52241715399616</v>
-      </c>
-      <c r="D29" s="19"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>24</v>
-      </c>
-      <c r="B30">
-        <v>1351.865</v>
-      </c>
-      <c r="C30">
-        <v>114.42495126705646</v>
-      </c>
-      <c r="D30" s="19"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>25</v>
-      </c>
-      <c r="B31">
-        <v>1302.6000000000001</v>
-      </c>
-      <c r="C31">
-        <v>114.52241715399616</v>
-      </c>
-      <c r="D31" s="19"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>26</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32" s="19"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>27</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33" s="19"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>28</v>
-      </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34" s="19"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>29</v>
-      </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35" s="19"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36" s="10"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="18" t="s">
+      <c r="D37" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3841,7 +3626,7 @@
       <c r="C38">
         <v>0.7</v>
       </c>
-      <c r="D38" s="19"/>
+      <c r="D38" s="13"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
@@ -3853,7 +3638,7 @@
       <c r="C39" s="5">
         <v>1.93</v>
       </c>
-      <c r="D39" s="19"/>
+      <c r="D39" s="13"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
@@ -3865,7 +3650,7 @@
       <c r="C40" s="7">
         <v>1.6</v>
       </c>
-      <c r="D40" s="19"/>
+      <c r="D40" s="13"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -3874,7 +3659,7 @@
       <c r="B41" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="19"/>
+      <c r="D41" s="13"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
@@ -3886,7 +3671,7 @@
       <c r="C42">
         <v>0</v>
       </c>
-      <c r="D42" s="19"/>
+      <c r="D42" s="13"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
@@ -3898,7 +3683,7 @@
       <c r="C43">
         <v>0</v>
       </c>
-      <c r="D43" s="19"/>
+      <c r="D43" s="13"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
@@ -3910,7 +3695,7 @@
       <c r="C44">
         <v>0</v>
       </c>
-      <c r="D44" s="19"/>
+      <c r="D44" s="13"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
@@ -3922,7 +3707,7 @@
       <c r="C45">
         <v>0.03</v>
       </c>
-      <c r="D45" s="19"/>
+      <c r="D45" s="13"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
@@ -3934,7 +3719,7 @@
       <c r="C46">
         <v>0.06</v>
       </c>
-      <c r="D46" s="19"/>
+      <c r="D46" s="13"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
@@ -3946,7 +3731,7 @@
       <c r="C47">
         <v>0.08</v>
       </c>
-      <c r="D47" s="19"/>
+      <c r="D47" s="13"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
@@ -3958,7 +3743,7 @@
       <c r="C48">
         <v>0.13</v>
       </c>
-      <c r="D48" s="19"/>
+      <c r="D48" s="13"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
@@ -3970,7 +3755,7 @@
       <c r="C49">
         <v>0.19</v>
       </c>
-      <c r="D49" s="19"/>
+      <c r="D49" s="13"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
@@ -3982,7 +3767,7 @@
       <c r="C50">
         <v>0.26</v>
       </c>
-      <c r="D50" s="19"/>
+      <c r="D50" s="13"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
@@ -3994,7 +3779,7 @@
       <c r="C51">
         <v>0.35</v>
       </c>
-      <c r="D51" s="19"/>
+      <c r="D51" s="13"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
@@ -4006,7 +3791,7 @@
       <c r="C52">
         <v>0.46</v>
       </c>
-      <c r="D52" s="19"/>
+      <c r="D52" s="13"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
@@ -4018,7 +3803,7 @@
       <c r="C53">
         <v>0.6</v>
       </c>
-      <c r="D53" s="19"/>
+      <c r="D53" s="13"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
@@ -4030,7 +3815,7 @@
       <c r="C54">
         <v>0.7</v>
       </c>
-      <c r="D54" s="19"/>
+      <c r="D54" s="13"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
@@ -4042,7 +3827,7 @@
       <c r="C55">
         <v>0.7</v>
       </c>
-      <c r="D55" s="19"/>
+      <c r="D55" s="13"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
@@ -4054,7 +3839,7 @@
       <c r="C56">
         <v>0.7</v>
       </c>
-      <c r="D56" s="19"/>
+      <c r="D56" s="13"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
@@ -4066,7 +3851,7 @@
       <c r="C57">
         <v>0.7</v>
       </c>
-      <c r="D57" s="19"/>
+      <c r="D57" s="13"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
@@ -4078,7 +3863,7 @@
       <c r="C58">
         <v>0</v>
       </c>
-      <c r="D58" s="19"/>
+      <c r="D58" s="13"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
@@ -4090,7 +3875,7 @@
       <c r="C59">
         <v>0</v>
       </c>
-      <c r="D59" s="19"/>
+      <c r="D59" s="13"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
@@ -4102,7 +3887,7 @@
       <c r="C60">
         <v>0</v>
       </c>
-      <c r="D60" s="19"/>
+      <c r="D60" s="13"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
@@ -4114,7 +3899,7 @@
       <c r="C61">
         <v>0</v>
       </c>
-      <c r="D61" s="19"/>
+      <c r="D61" s="13"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
@@ -4126,7 +3911,7 @@
       <c r="C62">
         <v>0</v>
       </c>
-      <c r="D62" s="19"/>
+      <c r="D62" s="13"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
@@ -4138,7 +3923,7 @@
       <c r="C63">
         <v>0</v>
       </c>
-      <c r="D63" s="19"/>
+      <c r="D63" s="13"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
@@ -4150,7 +3935,7 @@
       <c r="C64">
         <v>0</v>
       </c>
-      <c r="D64" s="19"/>
+      <c r="D64" s="13"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
@@ -4162,7 +3947,7 @@
       <c r="C65">
         <v>0</v>
       </c>
-      <c r="D65" s="19"/>
+      <c r="D65" s="13"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
@@ -4174,7 +3959,7 @@
       <c r="C66">
         <v>0</v>
       </c>
-      <c r="D66" s="19"/>
+      <c r="D66" s="13"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
@@ -4186,7 +3971,7 @@
       <c r="C67">
         <v>0</v>
       </c>
-      <c r="D67" s="19"/>
+      <c r="D67" s="13"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
@@ -4198,7 +3983,7 @@
       <c r="C68">
         <v>0</v>
       </c>
-      <c r="D68" s="19"/>
+      <c r="D68" s="13"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
@@ -4210,7 +3995,7 @@
       <c r="C69">
         <v>0</v>
       </c>
-      <c r="D69" s="19"/>
+      <c r="D69" s="13"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
@@ -4222,7 +4007,7 @@
       <c r="C70">
         <v>0</v>
       </c>
-      <c r="D70" s="19"/>
+      <c r="D70" s="13"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
@@ -4234,7 +4019,7 @@
       <c r="C71">
         <v>0</v>
       </c>
-      <c r="D71" s="19"/>
+      <c r="D71" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>